<commit_message>
add flask-blogly part 1
</commit_message>
<xml_diff>
--- a/sql-ddl-design/part2/part2_ddl_designs.xlsx
+++ b/sql-ddl-design/part2/part2_ddl_designs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karenrusseth/Desktop/dev-repo/sql-ddl-design/part2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B5AA91-4903-6D48-BAA6-18DFD52C68E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DBD58C-EEE4-0248-B438-C83FB73B62B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="1640" windowWidth="25180" windowHeight="16380" activeTab="1" xr2:uid="{20CBC6DB-FB33-994C-B7B2-4589F3051648}"/>
+    <workbookView xWindow="6080" yWindow="2360" windowWidth="25180" windowHeight="16380" activeTab="1" xr2:uid="{20CBC6DB-FB33-994C-B7B2-4589F3051648}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -102,15 +102,15 @@
     <t>Airports</t>
   </si>
   <si>
-    <t>Tickets</t>
-  </si>
-  <si>
     <t>first_name</t>
   </si>
   <si>
     <t>last_name</t>
   </si>
   <si>
+    <t>Flights</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -147,9 +147,6 @@
     <t>to_country</t>
   </si>
   <si>
-    <t>telephone</t>
-  </si>
-  <si>
     <t>airline_name</t>
   </si>
   <si>
@@ -159,7 +156,22 @@
     <t>airport_id</t>
   </si>
   <si>
+    <t>passenger_id</t>
+  </si>
+  <si>
     <t>airline_id</t>
+  </si>
+  <si>
+    <t>hub_city</t>
+  </si>
+  <si>
+    <t>flight_num</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>flight_id</t>
   </si>
 </sst>
 </file>
@@ -183,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -226,6 +238,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -248,12 +266,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -262,6 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -824,38 +844,38 @@
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -866,14 +886,14 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" t="s">
         <v>0</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="9"/>
+      <c r="I3" s="10"/>
       <c r="J3" t="s">
         <v>0</v>
       </c>
@@ -885,33 +905,33 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="I4" s="10"/>
       <c r="J4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="4"/>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F9" t="s">
@@ -927,7 +947,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>4</v>
       </c>
       <c r="F11" t="s">
@@ -961,10 +981,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530FA536-3435-BB46-A912-201BEDEE82E1}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,31 +996,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" s="5"/>
+      <c r="D1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E1" s="14"/>
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
+      <c r="H1" s="1"/>
+      <c r="J1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -1008,84 +1032,108 @@
       <c r="H2" t="s">
         <v>40</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K10" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K11" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="K12" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>